<commit_message>
Created monsterfactory, attack overrides
To do:
Goblin attack override
Limit user input
</commit_message>
<xml_diff>
--- a/Timeplan.xlsx
+++ b/Timeplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SAE\Projects\MonsterFight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68E4A58-04C2-4910-96DA-A2B09C2B9C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AC3534-7D4D-48D7-B89F-1BCB15C36A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25500" yWindow="0" windowWidth="25800" windowHeight="21705" xr2:uid="{939A5B08-884D-4DE7-B9EC-74919C1A4D6E}"/>
+    <workbookView xWindow="32070" yWindow="2985" windowWidth="16980" windowHeight="10155" xr2:uid="{939A5B08-884D-4DE7-B9EC-74919C1A4D6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Milestone</t>
   </si>
@@ -63,13 +63,7 @@
     <t>Sum</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>Override attack methods for races</t>
   </si>
 </sst>
 </file>
@@ -509,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48694031-7F89-4135-B74E-7F91D0658A5F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -591,22 +585,33 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
-        <f t="shared" ref="B7:C7" si="0">SUM(B2:B6)</f>
-        <v>170</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="6">
+        <f>SUM(B2:B7)</f>
+        <v>230</v>
+      </c>
+      <c r="C8" s="6">
+        <f>SUM(C2:C7)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>